<commit_message>
Added few more error and success codes.
git-svn-id: https://meridianww.cloudapp.net/svn/M4PL/trunk@5319 80c1dc9e-45f0-9747-8a74-c6ecc499fc54
</commit_message>
<xml_diff>
--- a/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
+++ b/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
   <si>
     <t>Success - 1</t>
   </si>
@@ -59,7 +59,7 @@
     <t>ShippingScheduleRequest / ShippingScheduleHeader</t>
   </si>
   <si>
-    <t>Created CSV</t>
+    <t>Created Local CSV</t>
   </si>
   <si>
     <t>PurposeCoded</t>
@@ -86,7 +86,7 @@
     <t>Create CSV</t>
   </si>
   <si>
-    <t>Deleted CreatedFile</t>
+    <t>Deleted Local File</t>
   </si>
   <si>
     <t>Name1</t>
@@ -95,6 +95,9 @@
     <t>Create XML</t>
   </si>
   <si>
+    <t xml:space="preserve">Uploaded File Locally </t>
+  </si>
+  <si>
     <t>Street</t>
   </si>
   <si>
@@ -120,6 +123,9 @@
   </si>
   <si>
     <t>RegionCoded</t>
+  </si>
+  <si>
+    <t>UploadToLocalPath</t>
   </si>
   <si>
     <t>ContactName</t>
@@ -309,8 +315,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -335,9 +341,36 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -353,7 +386,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,7 +431,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -385,59 +456,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,30 +469,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,13 +506,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,169 +662,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,30 +783,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -816,6 +798,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -826,6 +828,30 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -854,32 +880,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -897,134 +903,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1059,18 +1065,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1091,12 +1097,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1424,27 +1424,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S67"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" style="14" customWidth="1"/>
-    <col min="2" max="2" width="9.85714285714286" style="15" customWidth="1"/>
+    <col min="1" max="1" width="23" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.85714285714286" style="13" customWidth="1"/>
     <col min="4" max="4" width="9.14285714285714" style="16"/>
-    <col min="6" max="6" width="40" style="14" customWidth="1"/>
-    <col min="7" max="7" width="9.85714285714286" style="15" customWidth="1"/>
+    <col min="6" max="6" width="40" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.85714285714286" style="13" customWidth="1"/>
     <col min="10" max="10" width="9.14285714285714" style="16"/>
-    <col min="12" max="12" width="49.7142857142857" style="14" customWidth="1"/>
-    <col min="13" max="13" width="9.85714285714286" style="15" customWidth="1"/>
+    <col min="12" max="12" width="49.7142857142857" style="12" customWidth="1"/>
+    <col min="13" max="13" width="9.85714285714286" style="13" customWidth="1"/>
     <col min="16" max="16" width="9.14285714285714" style="16"/>
     <col min="19" max="19" width="21.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" ht="15.75" spans="1:19">
+    <row r="1" s="15" customFormat="1" ht="15.75" spans="1:19">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="19"/>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="18" t="s">
@@ -1471,12 +1471,12 @@
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
       <c r="P1" s="19"/>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="19" customHeight="1" spans="19:19">
-      <c r="S2" s="15">
+      <c r="S2" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       <c r="G6" s="22">
         <v>3</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="24" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="11">
@@ -1573,7 +1573,7 @@
       <c r="G7" s="22">
         <v>4</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="11">
@@ -1620,15 +1620,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="6:13">
+    <row r="10" customHeight="1" spans="1:13">
+      <c r="A10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
       <c r="F10" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="22">
         <v>7</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M10" s="11">
         <v>8</v>
@@ -1636,13 +1642,13 @@
     </row>
     <row r="11" spans="6:13">
       <c r="F11" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="22">
         <v>8</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M11" s="11">
         <v>9</v>
@@ -1650,43 +1656,49 @@
     </row>
     <row r="12" ht="17" customHeight="1" spans="6:13">
       <c r="F12" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="22">
         <v>9</v>
       </c>
-      <c r="L12" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="15">
+      <c r="L12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="6:13">
       <c r="F13" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" s="22">
         <v>10</v>
       </c>
-      <c r="L13" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="15">
+      <c r="L13" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="6:7">
+    <row r="14" spans="6:13">
       <c r="F14" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G14" s="22">
         <v>11</v>
       </c>
+      <c r="L14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="13">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="6:7">
       <c r="F15" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15" s="22">
         <v>12</v>
@@ -1694,7 +1706,7 @@
     </row>
     <row r="16" spans="6:7">
       <c r="F16" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G16" s="22">
         <v>13</v>
@@ -1702,247 +1714,83 @@
     </row>
     <row r="17" spans="6:7">
       <c r="F17" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G17" s="22">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="6:7">
-      <c r="F18" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="15">
+      <c r="F18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="6:7">
-      <c r="F19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="F19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="6:7">
-      <c r="F20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="15">
+      <c r="F20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="6:7">
-      <c r="F21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="15">
+      <c r="F21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="13">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="6:7">
-      <c r="F22" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="15">
+      <c r="F22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="13">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="6:7">
-      <c r="F23" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="15">
+      <c r="F23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="6:7">
-      <c r="F24" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="15">
+      <c r="F24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="13">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="6:7">
-      <c r="F25" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="24">
+      <c r="F25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="13">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="6:7">
-      <c r="F26" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="24">
+      <c r="F26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="13">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="6:7">
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="28" spans="6:7">
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-    </row>
-    <row r="29" spans="6:7">
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
-    </row>
-    <row r="30" spans="6:7">
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
-    </row>
-    <row r="31" spans="6:7">
-      <c r="F31" s="23"/>
-      <c r="G31" s="24"/>
-    </row>
-    <row r="32" spans="6:7">
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
-    </row>
-    <row r="33" spans="6:7">
-      <c r="F33" s="23"/>
-      <c r="G33" s="24"/>
-    </row>
-    <row r="34" spans="6:7">
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="6:7">
-      <c r="F35" s="23"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="6:7">
-      <c r="F36" s="23"/>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="6:7">
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
-    </row>
-    <row r="38" spans="6:7">
-      <c r="F38" s="23"/>
-      <c r="G38" s="24"/>
-    </row>
-    <row r="39" spans="6:7">
-      <c r="F39" s="23"/>
-      <c r="G39" s="24"/>
-    </row>
-    <row r="40" spans="6:7">
-      <c r="F40" s="23"/>
-      <c r="G40" s="24"/>
-    </row>
-    <row r="41" spans="6:7">
-      <c r="F41" s="23"/>
-      <c r="G41" s="24"/>
-    </row>
-    <row r="42" spans="6:7">
-      <c r="F42" s="23"/>
-      <c r="G42" s="24"/>
-    </row>
-    <row r="43" spans="6:7">
-      <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
-    </row>
-    <row r="44" spans="6:7">
-      <c r="F44" s="23"/>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="45" spans="6:7">
-      <c r="F45" s="23"/>
-      <c r="G45" s="24"/>
-    </row>
-    <row r="46" spans="6:7">
-      <c r="F46" s="23"/>
-      <c r="G46" s="24"/>
-    </row>
-    <row r="47" spans="6:7">
-      <c r="F47" s="23"/>
-      <c r="G47" s="24"/>
-    </row>
-    <row r="48" spans="6:7">
-      <c r="F48" s="23"/>
-      <c r="G48" s="24"/>
-    </row>
-    <row r="49" spans="6:7">
-      <c r="F49" s="23"/>
-      <c r="G49" s="24"/>
-    </row>
-    <row r="50" spans="6:7">
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
-    </row>
-    <row r="51" spans="6:7">
-      <c r="F51" s="23"/>
-      <c r="G51" s="24"/>
-    </row>
-    <row r="52" spans="6:7">
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
-    </row>
-    <row r="53" spans="6:7">
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
-    </row>
-    <row r="54" spans="6:7">
-      <c r="F54" s="23"/>
-      <c r="G54" s="24"/>
-    </row>
-    <row r="55" spans="6:7">
-      <c r="F55" s="23"/>
-      <c r="G55" s="24"/>
-    </row>
-    <row r="56" spans="6:7">
-      <c r="F56" s="23"/>
-      <c r="G56" s="24"/>
-    </row>
-    <row r="57" spans="6:7">
-      <c r="F57" s="23"/>
-      <c r="G57" s="24"/>
-    </row>
-    <row r="58" spans="6:7">
-      <c r="F58" s="23"/>
-      <c r="G58" s="24"/>
-    </row>
-    <row r="59" spans="6:7">
-      <c r="F59" s="23"/>
-      <c r="G59" s="24"/>
-    </row>
-    <row r="60" spans="6:7">
-      <c r="F60" s="23"/>
-      <c r="G60" s="24"/>
-    </row>
-    <row r="61" spans="6:7">
-      <c r="F61" s="23"/>
-      <c r="G61" s="24"/>
-    </row>
-    <row r="62" spans="6:7">
-      <c r="F62" s="23"/>
-      <c r="G62" s="24"/>
-    </row>
-    <row r="63" spans="6:7">
-      <c r="F63" s="23"/>
-      <c r="G63" s="24"/>
-    </row>
-    <row r="64" spans="6:7">
-      <c r="F64" s="23"/>
-      <c r="G64" s="24"/>
-    </row>
-    <row r="65" spans="6:7">
-      <c r="F65" s="23"/>
-      <c r="G65" s="24"/>
-    </row>
-    <row r="66" spans="6:7">
-      <c r="F66" s="23"/>
-      <c r="G66" s="24"/>
-    </row>
-    <row r="67" spans="6:7">
-      <c r="F67" s="23"/>
-      <c r="G67" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -1956,7 +1804,7 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2032,27 +1880,20 @@
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="2"/>
       <c r="F3" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="2"/>
       <c r="L3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="11">
         <v>0</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
       <c r="P3" s="5"/>
     </row>
     <row r="4" s="2" customFormat="1" customHeight="1" spans="1:16">
@@ -2062,27 +1903,20 @@
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
       <c r="F4" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="2"/>
       <c r="L4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="11">
         <v>1</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" s="2" customFormat="1" customHeight="1" spans="1:16">
@@ -2092,27 +1926,20 @@
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
       <c r="F5" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" s="4">
         <v>3</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="2"/>
       <c r="L5" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M5" s="11">
         <v>2</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
       <c r="P5" s="5"/>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:16">
@@ -2122,27 +1949,20 @@
       <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
       <c r="F6" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G6" s="4">
         <v>4</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="12" t="s">
-        <v>52</v>
+      <c r="L6" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="M6" s="11">
         <v>3</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="16" customHeight="1" spans="1:16">
@@ -2152,27 +1972,20 @@
       <c r="B7" s="11">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G7" s="4">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="2"/>
       <c r="L7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="11">
         <v>4</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:16">
@@ -2182,27 +1995,20 @@
       <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="4">
         <v>6</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="2"/>
       <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="11">
         <v>6</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
       <c r="P8" s="5"/>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:16">
@@ -2212,343 +2018,246 @@
       <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="2"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="2"/>
       <c r="L9" s="10" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="11">
         <v>7</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" s="2" customFormat="1" customHeight="1" spans="1:16">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4">
         <v>8</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="2"/>
       <c r="L10" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M10" s="11">
         <v>8</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
       <c r="P10" s="5"/>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:16">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="2"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4">
         <v>9</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="2"/>
       <c r="L11" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M11" s="11">
         <v>9</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
       <c r="P11" s="5"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="17" customHeight="1" spans="1:16">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="2"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G12" s="4">
         <v>10</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="L12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="13">
+        <v>12</v>
+      </c>
       <c r="P12" s="5"/>
     </row>
     <row r="13" s="2" customFormat="1" customHeight="1" spans="1:16">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="2"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
       <c r="F13" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G13" s="4">
         <v>11</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="2"/>
       <c r="L13" s="3"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
       <c r="P13" s="5"/>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:16">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="2"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="2"/>
       <c r="L14" s="3"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
       <c r="P14" s="5"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1" spans="1:16">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G15" s="4">
         <v>13</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="2"/>
       <c r="L15" s="3"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
       <c r="P15" s="5"/>
     </row>
     <row r="16" s="2" customFormat="1" spans="1:16">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="2"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G16" s="4">
         <v>14</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="2"/>
       <c r="L16" s="3"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
       <c r="P16" s="5"/>
     </row>
     <row r="17" s="2" customFormat="1" spans="1:16">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="2"/>
       <c r="F17" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G17" s="4">
         <v>15</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="2"/>
       <c r="L17" s="3"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
       <c r="P17" s="5"/>
     </row>
     <row r="18" s="2" customFormat="1" spans="1:16">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="2"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="2"/>
       <c r="F18" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G18" s="4">
         <v>16</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="2"/>
       <c r="L18" s="3"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
       <c r="P18" s="5"/>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:16">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="2"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G19" s="4">
         <v>17</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
       <c r="P19" s="5"/>
     </row>
     <row r="20" s="2" customFormat="1" spans="1:16">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="2"/>
       <c r="F20" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G20" s="4">
         <v>18</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
       <c r="P20" s="5"/>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:16">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="2"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="2"/>
       <c r="F21" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G21" s="4">
         <v>19</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="2"/>
       <c r="L21" s="3"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
       <c r="P21" s="5"/>
     </row>
     <row r="22" s="2" customFormat="1" spans="1:16">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="2"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="2"/>
       <c r="F22" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G22" s="4">
         <v>20</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="2"/>
       <c r="L22" s="3"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
       <c r="P22" s="5"/>
     </row>
     <row r="23" s="2" customFormat="1" spans="1:16">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="2"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="2"/>
       <c r="F23" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G23" s="4">
         <v>21</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="2"/>
       <c r="L23" s="3"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
       <c r="P23" s="5"/>
     </row>
     <row r="24" s="2" customFormat="1" spans="1:16">
@@ -2556,7 +2265,7 @@
       <c r="B24" s="4"/>
       <c r="D24" s="5"/>
       <c r="F24" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G24" s="4">
         <v>22</v>
@@ -2569,595 +2278,406 @@
     <row r="25" s="2" customFormat="1" spans="1:16">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="2"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
       <c r="F25" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G25" s="4">
         <v>23</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="2"/>
       <c r="L25" s="3"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
       <c r="P25" s="5"/>
     </row>
     <row r="26" s="2" customFormat="1" spans="1:16">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="2"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="2"/>
       <c r="F26" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G26" s="4">
         <v>24</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="2"/>
       <c r="L26" s="3"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
       <c r="P26" s="5"/>
     </row>
     <row r="27" s="2" customFormat="1" spans="1:16">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="2"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="2"/>
       <c r="F27" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G27" s="4">
         <v>25</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="2"/>
       <c r="L27" s="3"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
       <c r="P27" s="5"/>
     </row>
     <row r="28" s="2" customFormat="1" spans="1:16">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="2"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="2"/>
       <c r="F28" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G28" s="4">
         <v>26</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="2"/>
       <c r="L28" s="3"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
       <c r="P28" s="5"/>
     </row>
     <row r="29" s="2" customFormat="1" spans="1:16">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="2"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="2"/>
       <c r="F29" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G29" s="4">
         <v>27</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="2"/>
       <c r="L29" s="3"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
       <c r="P29" s="5"/>
     </row>
     <row r="30" s="2" customFormat="1" spans="1:16">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="2"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G30" s="4">
         <v>28</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="2"/>
       <c r="L30" s="3"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
       <c r="P30" s="5"/>
     </row>
     <row r="31" s="2" customFormat="1" spans="1:16">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="2"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="2"/>
       <c r="F31" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G31" s="4">
         <v>29</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="2"/>
       <c r="L31" s="3"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
       <c r="P31" s="5"/>
     </row>
     <row r="32" s="2" customFormat="1" spans="1:16">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="2"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="2"/>
       <c r="F32" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G32" s="4">
         <v>30</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
       <c r="P32" s="5"/>
     </row>
     <row r="33" s="2" customFormat="1" spans="1:16">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="2"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="2"/>
       <c r="F33" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G33" s="4">
         <v>31</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
       <c r="P33" s="5"/>
     </row>
     <row r="34" s="2" customFormat="1" spans="1:16">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="2"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="2"/>
       <c r="F34" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G34" s="4">
         <v>32</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="2"/>
       <c r="L34" s="3"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
       <c r="P34" s="5"/>
     </row>
     <row r="35" s="2" customFormat="1" spans="1:16">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="2"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="2"/>
       <c r="F35" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G35" s="4">
         <v>33</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="2"/>
       <c r="L35" s="3"/>
       <c r="M35" s="4"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
       <c r="P35" s="5"/>
     </row>
     <row r="36" s="2" customFormat="1" spans="1:16">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="2"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="2"/>
       <c r="F36" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G36" s="4">
         <v>34</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="2"/>
       <c r="L36" s="3"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
       <c r="P36" s="5"/>
     </row>
     <row r="37" s="2" customFormat="1" spans="1:16">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="2"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="2"/>
       <c r="F37" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G37" s="4">
         <v>35</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="2"/>
       <c r="L37" s="3"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
       <c r="P37" s="5"/>
     </row>
     <row r="38" s="2" customFormat="1" spans="1:16">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="2"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="2"/>
       <c r="F38" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G38" s="4">
         <v>36</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="2"/>
       <c r="L38" s="3"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
       <c r="P38" s="5"/>
     </row>
     <row r="39" s="2" customFormat="1" spans="1:16">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="2"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="2"/>
       <c r="F39" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G39" s="4">
         <v>37</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
       <c r="P39" s="5"/>
     </row>
     <row r="40" s="2" customFormat="1" spans="1:16">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="2"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="2"/>
       <c r="F40" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G40" s="4">
         <v>38</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="2"/>
       <c r="L40" s="3"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
       <c r="P40" s="5"/>
     </row>
     <row r="41" s="2" customFormat="1" spans="1:16">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="2"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="2"/>
       <c r="F41" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G41" s="4">
         <v>39</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="2"/>
       <c r="L41" s="3"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
       <c r="P41" s="5"/>
     </row>
     <row r="42" s="2" customFormat="1" spans="1:16">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="2"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="2"/>
       <c r="F42" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G42" s="4">
         <v>40</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="2"/>
       <c r="L42" s="3"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
       <c r="P42" s="5"/>
     </row>
     <row r="43" s="2" customFormat="1" spans="1:16">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="2"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="2"/>
       <c r="F43" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G43" s="4">
         <v>41</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="2"/>
       <c r="L43" s="3"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
       <c r="P43" s="5"/>
     </row>
     <row r="44" s="2" customFormat="1" spans="1:16">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="2"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="2"/>
       <c r="F44" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G44" s="4">
         <v>42</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="2"/>
       <c r="L44" s="3"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
       <c r="P44" s="5"/>
     </row>
     <row r="45" s="2" customFormat="1" spans="1:16">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="2"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="2"/>
       <c r="F45" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G45" s="4">
         <v>43</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
       <c r="J45" s="5"/>
-      <c r="K45" s="2"/>
       <c r="L45" s="3"/>
       <c r="M45" s="4"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" s="2" customFormat="1" spans="1:16">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
-      <c r="C46" s="2"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="2"/>
       <c r="F46" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G46" s="4">
         <v>44</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="2"/>
       <c r="L46" s="3"/>
       <c r="M46" s="4"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
       <c r="P46" s="5"/>
     </row>
     <row r="47" s="2" customFormat="1" spans="1:16">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="2"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="2"/>
       <c r="F47" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G47" s="4">
         <v>45</v>
       </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="2"/>
       <c r="L47" s="3"/>
       <c r="M47" s="4"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
       <c r="P47" s="5"/>
     </row>
     <row r="48" s="2" customFormat="1" spans="1:16">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="2"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="2"/>
       <c r="F48" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G48" s="4">
         <v>46</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="2"/>
       <c r="L48" s="3"/>
       <c r="M48" s="4"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
       <c r="P48" s="5"/>
     </row>
     <row r="49" s="2" customFormat="1" spans="1:16">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="2"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="2"/>
       <c r="F49" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G49" s="4">
         <v>47</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="2"/>
       <c r="L49" s="3"/>
       <c r="M49" s="4"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
       <c r="P49" s="5"/>
     </row>
     <row r="50" s="2" customFormat="1" spans="1:16">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="2"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="2"/>
       <c r="F50" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G50" s="4">
         <v>48</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="2"/>
       <c r="L50" s="3"/>
       <c r="M50" s="4"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
       <c r="P50" s="5"/>
     </row>
     <row r="51" s="2" customFormat="1" spans="1:16">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="2"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="2"/>
       <c r="F51" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G51" s="4">
         <v>49</v>
       </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="4"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
       <c r="P51" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues raised by client.
git-svn-id: https://meridianww.cloudapp.net/svn/M4PL/trunk@5447 80c1dc9e-45f0-9747-8a74-c6ecc499fc54
</commit_message>
<xml_diff>
--- a/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
+++ b/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ShippingSchANDShippingSchResp" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118">
   <si>
     <t>Success - 1</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>SendShippingScheduleResponse</t>
+  </si>
+  <si>
+    <t>DownloadPBSOUTFolderFile</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -402,83 +405,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -501,11 +427,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -517,8 +482,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -533,14 +529,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -567,7 +570,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,25 +624,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,7 +642,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +684,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,13 +714,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,55 +738,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,43 +750,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,6 +847,71 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -871,73 +939,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -946,15 +949,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -964,130 +967,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2769,8 +2772,8 @@
   <sheetPr/>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3028,8 +3031,12 @@
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="8">
+        <v>8</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="14"/>

</xml_diff>

<commit_message>
added one error code for PBS logging.
git-svn-id: https://meridianww.cloudapp.net/svn/M4PL/trunk@5508 80c1dc9e-45f0-9747-8a74-c6ecc499fc54
</commit_message>
<xml_diff>
--- a/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
+++ b/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\M4PL_Project\XCBL_Codebase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="ShippingSchANDShippingSchResp" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Requisition" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ShippingScheduleResponseRequest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ShippingSchANDShippingSchResp" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisition" sheetId="2" r:id="rId2"/>
+    <sheet name="ShippingScheduleResponseRequest" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,414 +26,396 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
-  <si>
-    <t xml:space="preserve">Success - 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warning - 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error - 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB Connection Failed - 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Received Request</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="122">
+  <si>
+    <t>Success - 1</t>
+  </si>
+  <si>
+    <t>Sub Code</t>
+  </si>
+  <si>
+    <t>Warning - 2</t>
+  </si>
+  <si>
+    <t>Error - 3</t>
+  </si>
+  <si>
+    <t>DB Connection Failed - 0</t>
+  </si>
+  <si>
+    <t>Received Request</t>
   </si>
   <si>
     <t xml:space="preserve">Cannot retrieve record </t>
   </si>
   <si>
-    <t xml:space="preserve">Global</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthenticatedRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule Issue date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request parsed for csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScheduleReferences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShippingScheduleRequest / ShippingScheduleHeader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created Local CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PurposeCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScheduleId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created Xml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScheduleType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrderNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uploaded Created file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deleted Local File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create XML</t>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>AuthenticatedRequest</t>
+  </si>
+  <si>
+    <t>Schedule Issue date</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Request parsed for csv</t>
+  </si>
+  <si>
+    <t>ScheduleReferences</t>
+  </si>
+  <si>
+    <t>ShippingScheduleRequest / ShippingScheduleHeader</t>
+  </si>
+  <si>
+    <t>Created Local CSV</t>
+  </si>
+  <si>
+    <t>PurposeCoded</t>
+  </si>
+  <si>
+    <t>ScheduleId</t>
+  </si>
+  <si>
+    <t>Created Xml</t>
+  </si>
+  <si>
+    <t>ScheduleType</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
+  </si>
+  <si>
+    <t>Uploaded Created file</t>
+  </si>
+  <si>
+    <t>AgencyCoded</t>
+  </si>
+  <si>
+    <t>Create CSV</t>
+  </si>
+  <si>
+    <t>Deleted Local File</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Create XML</t>
   </si>
   <si>
     <t xml:space="preserve">Uploaded File Locally </t>
   </si>
   <si>
-    <t xml:space="preserve">Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UploadToFTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StreetSupplement1</t>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>UploadToFTP</t>
+  </si>
+  <si>
+    <t>StreetSupplement1</t>
   </si>
   <si>
     <t xml:space="preserve">Delele File either CSV or xml from hosted system </t>
   </si>
   <si>
-    <t xml:space="preserve">PostalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScheduleResponseID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShippingScheduleReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegionCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UploadToLocalPath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATE APPROVE/PENDING FLAGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListOfContactNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShippingInstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_GPSSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_Lattitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_LocationId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EstimatedArrivalDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScheduleResponseIssueDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refNum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResponseTypeCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Data from PBSWebService</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBS file line 2 values less then 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBS file linescount &lt; 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty PBS text file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionIssueDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionTypeCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionTypeCodedOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OtherRequisitionReferences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PurposeCodedOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionDates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequestedShipByDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequisitionParty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_NameAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_Name1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_StreetSupplement1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_PostalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipToParty_RegionCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_NameAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_Name1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_StreetSupplement1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_PostalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShipFromParty_RegionCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShippingInstructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TransportQuantities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListOfQuantityCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TransitDirection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TransitDirectionCoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TransitDirectionCodedOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TransportLocationList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_GPSCoordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_GPSSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTransportLocation_LocationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_GPSCoordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndTransportLocation_LocationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success - 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warning - 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error - 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Acknowledgement Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response Successful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saved PBS File In DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response Unsuccessful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty File in PBS FTP folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWC Response Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Shipping Schedule Request In DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CheckPBSFTPFolder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShippingScheduleId/OrderNumber/ResponseType/PurposeCoded Empty in PBS FTP file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SendShippingScheduleResponseRequestFromPBSFTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetShippingScheduleRequestFromDB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SendShippingScheduleResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DownloadPBSOUTFolderFile</t>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>ScheduleResponseID</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ShippingScheduleReference</t>
+  </si>
+  <si>
+    <t>RegionCoded</t>
+  </si>
+  <si>
+    <t>UploadToLocalPath</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>UPDATE APPROVE/PENDING FLAGS</t>
+  </si>
+  <si>
+    <t>ListOfContactNumber</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>ShippingInstruction</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_GPSSystem</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_Lattitude</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_Longitude</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_LocationId</t>
+  </si>
+  <si>
+    <t>EstimatedArrivalDate</t>
+  </si>
+  <si>
+    <t>ScheduleResponseIssueDate</t>
+  </si>
+  <si>
+    <t>refNum</t>
+  </si>
+  <si>
+    <t>ResponseTypeCoded</t>
+  </si>
+  <si>
+    <t>No Data from PBSWebService</t>
+  </si>
+  <si>
+    <t>PBS file line 2 values less then 29</t>
+  </si>
+  <si>
+    <t>PBS file linescount &lt; 2</t>
+  </si>
+  <si>
+    <t>Empty PBS text file</t>
+  </si>
+  <si>
+    <t>RequisitionIssueDate</t>
+  </si>
+  <si>
+    <t>RequisitionType</t>
+  </si>
+  <si>
+    <t>RequisitionTypeCoded</t>
+  </si>
+  <si>
+    <t>RequisitionRequest</t>
+  </si>
+  <si>
+    <t>RequisitionTypeCodedOther</t>
+  </si>
+  <si>
+    <t>RequisitionId</t>
+  </si>
+  <si>
+    <t>OtherRequisitionReferences</t>
+  </si>
+  <si>
+    <t>PurposeCodedOther</t>
+  </si>
+  <si>
+    <t>RequisitionDates</t>
+  </si>
+  <si>
+    <t>RequestedShipByDate</t>
+  </si>
+  <si>
+    <t>RequisitionParty</t>
+  </si>
+  <si>
+    <t>ShipToParty</t>
+  </si>
+  <si>
+    <t>ShipToParty_NameAddress</t>
+  </si>
+  <si>
+    <t>ShipToParty_Name1</t>
+  </si>
+  <si>
+    <t>ShipToParty_Street</t>
+  </si>
+  <si>
+    <t>ShipToParty_StreetSupplement1</t>
+  </si>
+  <si>
+    <t>ShipToParty_PostalCode</t>
+  </si>
+  <si>
+    <t>ShipToParty_City</t>
+  </si>
+  <si>
+    <t>ShipToParty_Region</t>
+  </si>
+  <si>
+    <t>ShipToParty_RegionCoded</t>
+  </si>
+  <si>
+    <t>ShipFromParty</t>
+  </si>
+  <si>
+    <t>ShipFromParty_NameAddress</t>
+  </si>
+  <si>
+    <t>ShipFromParty_Name1</t>
+  </si>
+  <si>
+    <t>ShipFromParty_Street</t>
+  </si>
+  <si>
+    <t>ShipFromParty_StreetSupplement1</t>
+  </si>
+  <si>
+    <t>ShipFromParty_PostalCode</t>
+  </si>
+  <si>
+    <t>ShipFromParty_City</t>
+  </si>
+  <si>
+    <t>ShipFromParty_Region</t>
+  </si>
+  <si>
+    <t>ShipFromParty_RegionCoded</t>
+  </si>
+  <si>
+    <t>ShippingInstructions</t>
+  </si>
+  <si>
+    <t>TransportQuantities</t>
+  </si>
+  <si>
+    <t>ListOfQuantityCoded</t>
+  </si>
+  <si>
+    <t>TransitDirection</t>
+  </si>
+  <si>
+    <t>TransitDirectionCoded</t>
+  </si>
+  <si>
+    <t>TransitDirectionCodedOther</t>
+  </si>
+  <si>
+    <t>TransportLocationList</t>
+  </si>
+  <si>
+    <t>StartTransportLocation</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_Location</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_GPSCoordinates</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_GPSSystem</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_Latitude</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_Longitude</t>
+  </si>
+  <si>
+    <t>StartTransportLocation_LocationID</t>
+  </si>
+  <si>
+    <t>EndTransportLocation</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_Location</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_GPSCoordinates</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_Latitude</t>
+  </si>
+  <si>
+    <t>EndTransportLocation_LocationID</t>
+  </si>
+  <si>
+    <t>Success - 4</t>
+  </si>
+  <si>
+    <t>Warning - 5</t>
+  </si>
+  <si>
+    <t>Error - 6</t>
+  </si>
+  <si>
+    <t>Created Request</t>
+  </si>
+  <si>
+    <t>No Acknowledgement Note</t>
+  </si>
+  <si>
+    <t>Response Successful</t>
+  </si>
+  <si>
+    <t>No Status</t>
+  </si>
+  <si>
+    <t>Saved PBS File In DB</t>
+  </si>
+  <si>
+    <t>Response Unsuccessful</t>
+  </si>
+  <si>
+    <t>Create Request</t>
+  </si>
+  <si>
+    <t>Empty File in PBS FTP folder</t>
+  </si>
+  <si>
+    <t>AWC Response Null</t>
+  </si>
+  <si>
+    <t>No Shipping Schedule Request In DB</t>
+  </si>
+  <si>
+    <t>CheckPBSFTPFolder</t>
+  </si>
+  <si>
+    <t>ShippingScheduleId/OrderNumber/ResponseType/PurposeCoded Empty in PBS FTP file</t>
+  </si>
+  <si>
+    <t>SendShippingScheduleResponseRequestFromPBSFTP</t>
+  </si>
+  <si>
+    <t>GetShippingScheduleRequestFromDB</t>
+  </si>
+  <si>
+    <t>SendShippingScheduleResponse</t>
+  </si>
+  <si>
+    <t>DownloadPBSOUTFolderFile</t>
+  </si>
+  <si>
+    <t>Create PBS Log</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -447,246 +433,491 @@
     </fill>
   </fills>
   <borders count="8">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="28">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="49.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="9.14"/>
+    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="40" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="49.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" customWidth="1"/>
+    <col min="20" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:19" s="7" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -717,405 +948,403 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="S2" s="2" t="n">
+    <row r="2" spans="1:19" ht="18.95" customHeight="1">
+      <c r="S2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:19">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="13">
         <v>0</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="11" t="n">
+      <c r="M3" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="11">
         <v>2</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="13">
         <v>1</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="11" t="n">
+      <c r="M4" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="13">
         <v>2</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="11" t="n">
+      <c r="M5" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:19">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="11">
         <v>4</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="13">
         <v>3</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="11" t="n">
+      <c r="M6" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:19" ht="15.95" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="11">
         <v>5</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="13" t="n">
+      <c r="G7" s="13">
         <v>4</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="11" t="n">
+      <c r="M7" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:19">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="11">
         <v>6</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="13">
         <v>5</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="11" t="n">
+      <c r="M8" s="11">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:19">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="11">
         <v>7</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="13" t="n">
+      <c r="G9" s="13">
         <v>6</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="M9" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:19" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="13">
         <v>7</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="11" t="n">
+      <c r="M10" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:19">
       <c r="F11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G11" s="13">
         <v>8</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="11" t="n">
+      <c r="M11" s="11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="F12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="13" t="n">
+      <c r="G12" s="13">
         <v>9</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="2" t="n">
+      <c r="M12" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:19" ht="15" customHeight="1">
       <c r="F13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="13" t="n">
+      <c r="G13" s="13">
         <v>10</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="M13" s="2" t="n">
+      <c r="M13" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:19">
       <c r="F14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="13" t="n">
+      <c r="G14" s="13">
         <v>11</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="M14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:19" ht="18" customHeight="1">
       <c r="F15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="13" t="n">
+      <c r="G15" s="13">
         <v>12</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="2" t="n">
+      <c r="M15" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:19">
       <c r="F16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="13" t="n">
+      <c r="G16" s="13">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
       <c r="F17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="13">
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="6:7">
       <c r="F18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="6:7">
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="6:7">
       <c r="F20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="6:7">
       <c r="F21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="6:7">
       <c r="F22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="6:7">
       <c r="F23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="6:7">
       <c r="F24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="6:7">
       <c r="F25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="6:7">
       <c r="F26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="6:7">
       <c r="F27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="6:7">
       <c r="F28" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="6:7">
       <c r="F29" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="6:7">
       <c r="F30" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="2">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:S51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="17" width="49.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="18" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="19" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="19" width="9.14"/>
+    <col min="1" max="1" width="23" style="17" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="40" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="18" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="49.7109375" style="17" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="18" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="19" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="20" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="19" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" style="19" customWidth="1"/>
+    <col min="20" max="1025" width="9.140625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:19" s="24" customFormat="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1146,545 +1375,537 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="S2" s="18" t="n">
+    <row r="2" spans="1:19" ht="18.95" customHeight="1">
+      <c r="S2" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:19">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="18" t="n">
+      <c r="G3" s="18">
         <v>1</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="11" t="n">
+      <c r="M3" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="11">
         <v>2</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="18" t="n">
+      <c r="G4" s="18">
         <v>2</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="11" t="n">
+      <c r="M4" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="18" t="n">
+      <c r="G5" s="18">
         <v>3</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="11" t="n">
+      <c r="M5" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:19">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="11">
         <v>4</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="18" t="n">
+      <c r="G6" s="18">
         <v>4</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="11" t="n">
+      <c r="M6" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:19" ht="15.95" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="11">
         <v>5</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="18" t="n">
+      <c r="G7" s="18">
         <v>5</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="11" t="n">
+      <c r="M7" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:19">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="11">
         <v>6</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18" t="n">
+      <c r="G8" s="18">
         <v>6</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="11" t="n">
+      <c r="M8" s="11">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:19">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="11">
         <v>7</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="18" t="n">
+      <c r="G9" s="18">
         <v>7</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="M9" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:19" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="18" t="n">
+      <c r="G10" s="18">
         <v>8</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="11" t="n">
+      <c r="M10" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:19">
       <c r="F11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="18" t="n">
+      <c r="G11" s="18">
         <v>9</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="11" t="n">
+      <c r="M11" s="11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="F12" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="18" t="n">
+      <c r="G12" s="18">
         <v>10</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="2" t="n">
+      <c r="M12" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:19" ht="15" customHeight="1">
       <c r="F13" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="18" t="n">
+      <c r="G13" s="18">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:19">
       <c r="F14" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="18" t="n">
+      <c r="G14" s="18">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:19" ht="18" customHeight="1">
       <c r="F15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="18" t="n">
+      <c r="G15" s="18">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:19">
       <c r="F16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="18" t="n">
+      <c r="G16" s="18">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="6:7">
       <c r="F17" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="18" t="n">
+      <c r="G17" s="18">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="6:7">
       <c r="F18" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G18" s="18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="6:7">
       <c r="F19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="18" t="n">
+      <c r="G19" s="18">
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="6:7">
       <c r="F20" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="18" t="n">
+      <c r="G20" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="6:7">
       <c r="F21" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="18" t="n">
+      <c r="G21" s="18">
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="6:7">
       <c r="F22" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="18">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="6:7">
       <c r="F23" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="18">
         <v>21</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="6:7">
       <c r="F24" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="18">
         <v>22</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="6:7">
       <c r="F25" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="18">
         <v>23</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="6:7">
       <c r="F26" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="18">
         <v>24</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="6:7">
       <c r="F27" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="18" t="n">
+      <c r="G27" s="18">
         <v>25</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="6:7">
       <c r="F28" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="18" t="n">
+      <c r="G28" s="18">
         <v>26</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="6:7">
       <c r="F29" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="18" t="n">
+      <c r="G29" s="18">
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="6:7">
       <c r="F30" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G30" s="18" t="n">
+      <c r="G30" s="18">
         <v>28</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="6:7">
       <c r="F31" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="18" t="n">
+      <c r="G31" s="18">
         <v>29</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="6:7">
       <c r="F32" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="18" t="n">
+      <c r="G32" s="18">
         <v>30</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="6:7">
       <c r="F33" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G33" s="18" t="n">
+      <c r="G33" s="18">
         <v>31</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="6:7">
       <c r="F34" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G34" s="18" t="n">
+      <c r="G34" s="18">
         <v>32</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="6:7">
       <c r="F35" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="18" t="n">
+      <c r="G35" s="18">
         <v>33</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="6:7">
       <c r="F36" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="18">
         <v>34</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="6:7">
       <c r="F37" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G37" s="18" t="n">
+      <c r="G37" s="18">
         <v>35</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="6:7">
       <c r="F38" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="G38" s="18" t="n">
+      <c r="G38" s="18">
         <v>36</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="6:7">
       <c r="F39" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="18" t="n">
+      <c r="G39" s="18">
         <v>37</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="6:7">
       <c r="F40" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="18" t="n">
+      <c r="G40" s="18">
         <v>38</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="6:7">
       <c r="F41" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="18" t="n">
+      <c r="G41" s="18">
         <v>39</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="6:7">
       <c r="F42" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="18" t="n">
+      <c r="G42" s="18">
         <v>40</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="6:7">
       <c r="F43" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="G43" s="18" t="n">
+      <c r="G43" s="18">
         <v>41</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="6:7">
       <c r="F44" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G44" s="18" t="n">
+      <c r="G44" s="18">
         <v>42</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="6:7">
       <c r="F45" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="18" t="n">
+      <c r="G45" s="18">
         <v>43</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="6:7">
       <c r="F46" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="G46" s="18" t="n">
+      <c r="G46" s="18">
         <v>44</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="6:7">
       <c r="F47" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G47" s="18" t="n">
+      <c r="G47" s="18">
         <v>45</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="6:7">
       <c r="F48" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G48" s="18" t="n">
+      <c r="G48" s="18">
         <v>46</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="6:7">
       <c r="F49" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G49" s="18" t="n">
+      <c r="G49" s="18">
         <v>47</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="6:7">
       <c r="F50" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G50" s="18" t="n">
+      <c r="G50" s="18">
         <v>48</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="6:7">
       <c r="F51" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G51" s="18" t="n">
+      <c r="G51" s="18">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="87.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="57.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="87.42578125" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="57.5703125" customWidth="1"/>
+    <col min="8" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:14">
       <c r="A1" s="21" t="s">
         <v>102</v>
       </c>
@@ -1712,7 +1933,7 @@
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:14">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
@@ -1728,25 +1949,25 @@
       <c r="M2" s="19"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:14">
       <c r="A3" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="18">
         <v>1</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="11" t="n">
+      <c r="H3" s="11">
         <v>0</v>
       </c>
       <c r="I3" s="19"/>
@@ -1756,25 +1977,25 @@
       <c r="M3" s="19"/>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:14">
       <c r="A4" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="11">
         <v>2</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="18">
         <v>2</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="11">
         <v>1</v>
       </c>
       <c r="I4" s="19"/>
@@ -1784,25 +2005,25 @@
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="18">
         <v>3</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="18" t="n">
+      <c r="H5" s="18">
         <v>2</v>
       </c>
       <c r="I5" s="19"/>
@@ -1812,21 +2033,21 @@
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:14">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="19"/>
       <c r="D6" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="18">
         <v>4</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="18" t="n">
+      <c r="H6" s="18">
         <v>3</v>
       </c>
       <c r="I6" s="19"/>
@@ -1836,21 +2057,21 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:14">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="19"/>
       <c r="D7" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="18">
         <v>5</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="11" t="n">
+      <c r="H7" s="11">
         <v>4</v>
       </c>
       <c r="I7" s="19"/>
@@ -1860,21 +2081,21 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:14">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="19"/>
       <c r="D8" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="18">
         <v>6</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="11" t="n">
+      <c r="H8" s="11">
         <v>5</v>
       </c>
       <c r="I8" s="19"/>
@@ -1884,7 +2105,7 @@
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:14">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="19"/>
@@ -1894,7 +2115,7 @@
       <c r="G9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="11" t="n">
+      <c r="H9" s="11">
         <v>6</v>
       </c>
       <c r="I9" s="19"/>
@@ -1904,7 +2125,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:14">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="19"/>
@@ -1914,7 +2135,7 @@
       <c r="G10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="11" t="n">
+      <c r="H10" s="11">
         <v>7</v>
       </c>
       <c r="I10" s="19"/>
@@ -1924,7 +2145,7 @@
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:14">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1934,7 +2155,7 @@
       <c r="G11" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="11" t="n">
+      <c r="H11" s="11">
         <v>8</v>
       </c>
       <c r="I11" s="19"/>
@@ -1944,7 +2165,7 @@
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:14">
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="17"/>
@@ -1959,7 +2180,7 @@
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:14">
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="17"/>
@@ -1974,7 +2195,7 @@
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:14">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1989,7 +2210,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:14">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -2004,7 +2225,7 @@
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:14">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -2020,7 +2241,7 @@
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:14">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -2036,7 +2257,7 @@
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:14">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -2052,7 +2273,7 @@
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:14">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -2068,7 +2289,7 @@
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:14">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -2084,7 +2305,7 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:14">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -2100,7 +2321,7 @@
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:14">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -2116,7 +2337,7 @@
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:14">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -2132,7 +2353,7 @@
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:14">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -2148,7 +2369,7 @@
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:14">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -2164,7 +2385,7 @@
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:14">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -2180,7 +2401,7 @@
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:14">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
@@ -2196,7 +2417,7 @@
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:14">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -2212,7 +2433,7 @@
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:14">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -2228,7 +2449,7 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:14">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -2244,7 +2465,7 @@
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:14">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -2260,7 +2481,7 @@
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:14">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -2276,7 +2497,7 @@
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:14">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -2292,7 +2513,7 @@
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:14">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -2308,7 +2529,7 @@
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:14">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
@@ -2324,7 +2545,7 @@
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:14">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
@@ -2340,7 +2561,7 @@
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:14">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="19"/>
@@ -2356,7 +2577,7 @@
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:14">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -2372,7 +2593,7 @@
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:14">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
@@ -2388,7 +2609,7 @@
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:14">
       <c r="A40" s="17"/>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
@@ -2405,12 +2626,7 @@
       <c r="N40" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some more codes in shipping schedule Success
git-svn-id: https://meridianww.cloudapp.net/svn/M4PL/trunk@5518 80c1dc9e-45f0-9747-8a74-c6ecc499fc54
</commit_message>
<xml_diff>
--- a/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
+++ b/M4PL.XCBL.WebService/XCBL.WebService/XCBLServiceLogCodes.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
   <si>
     <t>Success - 1</t>
   </si>
@@ -392,6 +392,15 @@
   </si>
   <si>
     <t>Create PBS Log</t>
+  </si>
+  <si>
+    <t>PbsFrequencyTimer_Elapsed</t>
+  </si>
+  <si>
+    <t>Inside GetAllOrder</t>
+  </si>
+  <si>
+    <t>Inside CheckPBSFTPFolder</t>
   </si>
 </sst>
 </file>
@@ -892,13 +901,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3" customWidth="1"/>
@@ -1114,6 +1123,12 @@
       </c>
     </row>
     <row r="11" spans="1:19">
+      <c r="A11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
       <c r="F11" s="12" t="s">
         <v>29</v>
       </c>
@@ -1128,6 +1143,12 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
       <c r="F12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1142,6 +1163,12 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
       <c r="F13" s="12" t="s">
         <v>33</v>
       </c>

</xml_diff>